<commit_message>
Updated part 3 output for report
</commit_message>
<xml_diff>
--- a/Part3/svo021_final/10k_output_1.xlsx
+++ b/Part3/svo021_final/10k_output_1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Desktop\Spring-2022\167\workspace\final\Part3\svo021_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{08E7754B-5320-4E30-9D67-D6C3912CCCD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5275F6-09F5-4AC0-B653-883B3D7032E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="part-00000-80bdb291-ce25-4e26-a" sheetId="1" r:id="rId1"/>
@@ -280,7 +280,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -833,6 +833,78 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ratios</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Common Names</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" baseline="0"/>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>02/21/2015 to 05/22/2015</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="1.0642351097076205E-4"/>
+          <c:y val="5.170630816959669E-3"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -884,6 +956,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -899,6 +976,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -914,6 +996,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -929,6 +1016,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -944,6 +1036,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -959,6 +1056,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -976,6 +1078,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -993,6 +1100,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -1010,6 +1122,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -1027,6 +1144,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -1044,6 +1166,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -1061,6 +1188,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -1079,6 +1211,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -1097,6 +1234,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -1115,6 +1257,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
@@ -1133,6 +1280,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="16"/>
@@ -1151,6 +1303,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="17"/>
@@ -1169,6 +1326,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="18"/>
@@ -1186,6 +1348,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="19"/>
@@ -1203,6 +1370,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000027-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="20"/>
@@ -1220,6 +1392,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000029-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="21"/>
@@ -1237,6 +1414,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002B-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="22"/>
@@ -1254,6 +1436,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002D-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="23"/>
@@ -1271,6 +1458,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002F-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="24"/>
@@ -1289,6 +1481,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000031-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="25"/>
@@ -1307,6 +1504,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000033-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="26"/>
@@ -1325,6 +1527,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000035-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="27"/>
@@ -1343,6 +1550,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000037-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="28"/>
@@ -1361,6 +1573,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000039-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="29"/>
@@ -1379,6 +1596,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003B-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="30"/>
@@ -1396,6 +1618,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003D-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="31"/>
@@ -1413,6 +1640,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003F-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="32"/>
@@ -1430,6 +1662,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000041-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="33"/>
@@ -1447,6 +1684,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000043-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="34"/>
@@ -1464,6 +1706,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000045-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="35"/>
@@ -1481,6 +1728,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000047-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="36"/>
@@ -1499,6 +1751,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000049-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="37"/>
@@ -1517,6 +1774,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004B-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="38"/>
@@ -1535,6 +1797,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004D-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="39"/>
@@ -1553,6 +1820,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004F-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="40"/>
@@ -1571,6 +1843,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000051-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="41"/>
@@ -1589,6 +1866,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000053-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="42"/>
@@ -1606,6 +1888,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000055-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="43"/>
@@ -1623,6 +1910,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000057-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="44"/>
@@ -1640,6 +1932,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000059-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="45"/>
@@ -1657,6 +1954,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005B-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="46"/>
@@ -1674,6 +1976,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005D-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="47"/>
@@ -1691,6 +1998,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000005F-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="48"/>
@@ -1709,6 +2021,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000061-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="49"/>
@@ -1727,6 +2044,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000063-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="50"/>
@@ -1745,6 +2067,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000065-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="51"/>
@@ -1763,6 +2090,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000067-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="52"/>
@@ -1781,6 +2113,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000069-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="53"/>
@@ -1799,6 +2136,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000006B-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="54"/>
@@ -1814,6 +2156,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000006D-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="55"/>
@@ -1829,6 +2176,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000006F-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="56"/>
@@ -1844,6 +2196,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000071-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="57"/>
@@ -1859,6 +2216,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000073-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="58"/>
@@ -1874,6 +2236,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000075-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="59"/>
@@ -1889,6 +2256,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000077-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="60"/>
@@ -1906,6 +2278,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000079-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="61"/>
@@ -1923,6 +2300,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000007B-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="62"/>
@@ -1940,6 +2322,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000007D-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="63"/>
@@ -1957,6 +2344,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000007F-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="64"/>
@@ -1974,6 +2366,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000081-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="65"/>
@@ -1991,6 +2388,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000083-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="66"/>
@@ -2009,6 +2411,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000085-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="67"/>
@@ -2027,6 +2434,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000087-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="68"/>
@@ -2045,6 +2457,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000089-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="69"/>
@@ -2063,6 +2480,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000008B-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="70"/>
@@ -2081,6 +2503,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000008D-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="71"/>
@@ -2099,6 +2526,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000008F-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="72"/>
@@ -2116,6 +2548,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000091-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="73"/>
@@ -2133,6 +2570,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000093-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="74"/>
@@ -2150,6 +2592,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000095-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="75"/>
@@ -2167,6 +2614,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000097-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="76"/>
@@ -2184,6 +2636,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000099-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="77"/>
@@ -2201,6 +2658,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000009B-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="78"/>
@@ -2219,6 +2681,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000009D-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="79"/>
@@ -2237,6 +2704,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000009F-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="80"/>
@@ -2255,6 +2727,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{000000A1-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="81"/>
@@ -2273,6 +2750,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{000000A3-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="82"/>
@@ -2291,6 +2773,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{000000A5-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="83"/>
@@ -2309,6 +2796,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{000000A7-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="84"/>
@@ -2326,6 +2818,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{000000A9-C37A-4C20-ACBD-6F3CDCA23AC6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -3904,16 +4401,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3921,7 +4418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3929,7 +4426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3937,7 +4434,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3945,7 +4442,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3953,7 +4450,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3961,7 +4458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3969,7 +4466,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3977,7 +4474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3985,7 +4482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3993,7 +4490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -4001,7 +4498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -4009,7 +4506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -4017,7 +4514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -4025,7 +4522,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -4033,7 +4530,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -4041,7 +4538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -4049,7 +4546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -4057,7 +4554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -4065,7 +4562,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -4073,7 +4570,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -4081,7 +4578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -4089,7 +4586,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -4097,7 +4594,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -4105,7 +4602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -4113,7 +4610,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -4121,7 +4618,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -4129,7 +4626,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -4137,7 +4634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -4145,7 +4642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -4153,7 +4650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -4161,7 +4658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -4169,7 +4666,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -4177,7 +4674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -4185,7 +4682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -4193,7 +4690,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -4201,7 +4698,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -4209,7 +4706,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -4217,7 +4714,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -4225,7 +4722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -4233,7 +4730,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -4241,7 +4738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -4249,7 +4746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -4257,7 +4754,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -4265,7 +4762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -4273,7 +4770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -4281,7 +4778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -4289,7 +4786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -4297,7 +4794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -4305,7 +4802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -4313,7 +4810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -4321,7 +4818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -4329,7 +4826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -4337,7 +4834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -4345,7 +4842,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -4353,7 +4850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -4361,7 +4858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -4369,7 +4866,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -4377,7 +4874,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -4385,7 +4882,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -4393,7 +4890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -4401,7 +4898,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -4409,7 +4906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -4417,7 +4914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -4425,7 +4922,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -4433,7 +4930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -4441,7 +4938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -4449,7 +4946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -4457,7 +4954,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -4465,7 +4962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -4473,7 +4970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -4481,7 +4978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -4489,7 +4986,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -4497,7 +4994,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -4505,12 +5002,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -4518,7 +5015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -4526,7 +5023,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -4534,7 +5031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -4542,7 +5039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -4550,7 +5047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -4558,7 +5055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -4566,7 +5063,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -4574,7 +5071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -4582,7 +5079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>

</xml_diff>